<commit_message>
Minor fixes to forms field labels
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-3CE.xlsx
+++ b/form_reporting_templates/Form-3CE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\Data dissemination\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB32962-77F0-4EA5-9BCC-69B91C36451F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEEC1BC-9F6D-4307-90DD-05957BCE1431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="JaUivJj1XpzVIsMUuIWG4pvRwNkhjECqAfRNMoS0pEzY8qCMrWJoKRkwK5J/dPq5W+eH0fv+0nU0ZPhh5rEo8w==" workbookSaltValue="WSrsrEWzygKOJ9WtcOLB6A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
@@ -879,15 +879,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2642,7 +2642,7 @@
       <c r="G55" s="39"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="xP/vU14SDPFSd5xl+n7X3arHM/pR8+OPREMT7TOexFwou0hgBtfvnNk51JZ9q46IALErKTYgvSdO2oRARzRvuw==" saltValue="SfsHgQE4R2XHMhOnBKlnTQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qu+HEgqrWIbEREl7p31mJI9r2dZa9xw/0VESHmIecIjlmCLVkKDarlXaDjhqLWi0PSX5uGEykLgI+0l9oJNcKA==" saltValue="ciFOWMQUNbWZnhDf/zBVZw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="B2:DC3"/>
     <mergeCell ref="E4:G4"/>

</xml_diff>